<commit_message>
initial cleaning and exploration
</commit_message>
<xml_diff>
--- a/Data/Concerns_Toward_Drug_Decriminalisation_and_Demographics_Data_Set.xlsx
+++ b/Data/Concerns_Toward_Drug_Decriminalisation_and_Demographics_Data_Set.xlsx
@@ -728,7 +728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -745,6 +745,15 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -760,14 +769,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10739,7 +10751,7 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="158" ht="14.25" customHeight="1">
+    <row r="158" ht="18.0" customHeight="1">
       <c r="A158" s="3" t="s">
         <v>175</v>
       </c>
@@ -10758,7 +10770,7 @@
       <c r="F158" s="1">
         <v>3.0</v>
       </c>
-      <c r="G158" s="1">
+      <c r="G158" s="4">
         <v>4.0</v>
       </c>
       <c r="H158" s="1">
@@ -10821,7 +10833,7 @@
         <v>8.0</v>
       </c>
       <c r="G159" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H159" s="1">
         <v>3.0</v>
@@ -10883,7 +10895,7 @@
         <v>9.0</v>
       </c>
       <c r="G160" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H160" s="1">
         <v>3.0</v>
@@ -10945,7 +10957,7 @@
         <v>1.0</v>
       </c>
       <c r="G161" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H161" s="1">
         <v>2.0</v>
@@ -11007,7 +11019,7 @@
         <v>1.0</v>
       </c>
       <c r="G162" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H162" s="1">
         <v>2.0</v>
@@ -11069,7 +11081,7 @@
         <v>1.0</v>
       </c>
       <c r="G163" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H163" s="1">
         <v>2.0</v>
@@ -11131,7 +11143,7 @@
         <v>1.0</v>
       </c>
       <c r="G164" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H164" s="1">
         <v>1.0</v>
@@ -11255,7 +11267,7 @@
         <v>2.0</v>
       </c>
       <c r="G166" s="1">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="H166" s="1">
         <v>3.0</v>
@@ -11317,7 +11329,7 @@
         <v>9.0</v>
       </c>
       <c r="G167" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H167" s="1">
         <v>3.0</v>
@@ -11441,7 +11453,7 @@
         <v>3.0</v>
       </c>
       <c r="G169" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H169" s="1">
         <v>1.0</v>
@@ -11503,7 +11515,7 @@
         <v>9.0</v>
       </c>
       <c r="G170" s="1">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H170" s="1">
         <v>3.0</v>
@@ -11565,7 +11577,7 @@
         <v>3.0</v>
       </c>
       <c r="G171" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H171" s="1">
         <v>3.0</v>
@@ -11689,7 +11701,7 @@
         <v>2.0</v>
       </c>
       <c r="G173" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H173" s="1">
         <v>2.0</v>
@@ -11751,7 +11763,7 @@
         <v>7.0</v>
       </c>
       <c r="G174" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H174" s="1">
         <v>1.0</v>
@@ -11813,7 +11825,7 @@
         <v>4.0</v>
       </c>
       <c r="G175" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H175" s="1">
         <v>1.0</v>
@@ -11875,7 +11887,7 @@
         <v>7.0</v>
       </c>
       <c r="G176" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H176" s="1">
         <v>3.0</v>
@@ -11937,7 +11949,7 @@
         <v>7.0</v>
       </c>
       <c r="G177" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H177" s="1">
         <v>1.0</v>
@@ -11999,7 +12011,7 @@
         <v>9.0</v>
       </c>
       <c r="G178" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H178" s="1">
         <v>3.0</v>
@@ -12061,7 +12073,7 @@
         <v>2.0</v>
       </c>
       <c r="G179" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H179" s="1">
         <v>1.0</v>
@@ -12123,7 +12135,7 @@
         <v>3.0</v>
       </c>
       <c r="G180" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H180" s="1">
         <v>3.0</v>
@@ -12185,7 +12197,7 @@
         <v>8.0</v>
       </c>
       <c r="G181" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H181" s="1">
         <v>2.0</v>
@@ -12247,7 +12259,7 @@
         <v>1.0</v>
       </c>
       <c r="G182" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H182" s="1">
         <v>1.0</v>
@@ -12433,7 +12445,7 @@
         <v>2.0</v>
       </c>
       <c r="G185" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H185" s="1">
         <v>3.0</v>
@@ -12495,7 +12507,7 @@
         <v>9.0</v>
       </c>
       <c r="G186" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H186" s="1">
         <v>3.0</v>
@@ -12557,7 +12569,7 @@
         <v>2.0</v>
       </c>
       <c r="G187" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H187" s="1">
         <v>3.0</v>
@@ -12619,7 +12631,7 @@
         <v>1.0</v>
       </c>
       <c r="G188" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H188" s="1">
         <v>3.0</v>
@@ -12681,7 +12693,7 @@
         <v>1.0</v>
       </c>
       <c r="G189" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H189" s="1">
         <v>3.0</v>
@@ -12805,7 +12817,7 @@
         <v>2.0</v>
       </c>
       <c r="G191" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="H191" s="1">
         <v>1.0</v>
@@ -12867,7 +12879,7 @@
         <v>4.0</v>
       </c>
       <c r="G192" s="1">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="H192" s="1">
         <v>3.0</v>
@@ -12991,7 +13003,7 @@
         <v>8.0</v>
       </c>
       <c r="G194" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="H194" s="1">
         <v>3.0</v>
@@ -13053,7 +13065,7 @@
         <v>7.0</v>
       </c>
       <c r="G195" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H195" s="1">
         <v>1.0</v>
@@ -13115,7 +13127,7 @@
         <v>3.0</v>
       </c>
       <c r="G196" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H196" s="1">
         <v>2.0</v>
@@ -13177,7 +13189,7 @@
         <v>7.0</v>
       </c>
       <c r="G197" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H197" s="1">
         <v>1.0</v>
@@ -13239,7 +13251,7 @@
         <v>2.0</v>
       </c>
       <c r="G198" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H198" s="1">
         <v>2.0</v>
@@ -13301,7 +13313,7 @@
         <v>2.0</v>
       </c>
       <c r="G199" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H199" s="1">
         <v>1.0</v>
@@ -13363,7 +13375,7 @@
         <v>1.0</v>
       </c>
       <c r="G200" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H200" s="1">
         <v>3.0</v>
@@ -13425,7 +13437,7 @@
         <v>9.0</v>
       </c>
       <c r="G201" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H201" s="1">
         <v>1.0</v>
@@ -13487,7 +13499,7 @@
         <v>7.0</v>
       </c>
       <c r="G202" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H202" s="1">
         <v>3.0</v>
@@ -13611,7 +13623,7 @@
         <v>9.0</v>
       </c>
       <c r="G204" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H204" s="1">
         <v>1.0</v>
@@ -13673,7 +13685,7 @@
         <v>1.0</v>
       </c>
       <c r="G205" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H205" s="1">
         <v>1.0</v>
@@ -13735,7 +13747,7 @@
         <v>1.0</v>
       </c>
       <c r="G206" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H206" s="1">
         <v>1.0</v>
@@ -13797,7 +13809,7 @@
         <v>9.0</v>
       </c>
       <c r="G207" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H207" s="1">
         <v>3.0</v>
@@ -13921,7 +13933,7 @@
         <v>1.0</v>
       </c>
       <c r="G209" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H209" s="1">
         <v>1.0</v>
@@ -13983,7 +13995,7 @@
         <v>4.0</v>
       </c>
       <c r="G210" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H210" s="1">
         <v>1.0</v>
@@ -14107,7 +14119,7 @@
         <v>7.0</v>
       </c>
       <c r="G212" s="1">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="H212" s="1">
         <v>3.0</v>
@@ -14169,7 +14181,7 @@
         <v>4.0</v>
       </c>
       <c r="G213" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="H213" s="1">
         <v>3.0</v>
@@ -14231,7 +14243,7 @@
         <v>8.0</v>
       </c>
       <c r="G214" s="1">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="H214" s="1">
         <v>1.0</v>
@@ -14293,7 +14305,7 @@
         <v>1.0</v>
       </c>
       <c r="G215" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H215" s="1">
         <v>3.0</v>
@@ -14355,7 +14367,7 @@
         <v>4.0</v>
       </c>
       <c r="G216" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H216" s="1">
         <v>1.0</v>
@@ -14417,7 +14429,7 @@
         <v>7.0</v>
       </c>
       <c r="G217" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H217" s="1">
         <v>1.0</v>
@@ -14479,7 +14491,7 @@
         <v>8.0</v>
       </c>
       <c r="G218" s="1">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H218" s="1">
         <v>3.0</v>

</xml_diff>